<commit_message>
change path to.py file
</commit_message>
<xml_diff>
--- a/examples/pca_decomposition/pca_decomposition.xlsx
+++ b/examples/pca_decomposition/pca_decomposition.xlsx
@@ -17,9 +17,6 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>n</t>
-  </si>
-  <si>
-    <t>D:\Users\Tandem Algorithms\My Development\GitHub\tdmalgorithms\examples\pca_decomposition\pca_decomposition.py</t>
   </si>
   <si>
     <t>cov</t>
@@ -56,6 +53,9 @@
   </si>
   <si>
     <t>RESULT</t>
+  </si>
+  <si>
+    <t>D:\Users\Tandem Algorithms\My Development\GitHub\tandem-algorithms\examples\pca_decomposition\pca_decomposition.py</t>
   </si>
 </sst>
 </file>
@@ -258,7 +258,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -278,7 +278,6 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -9560,11 +9559,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="225158272"/>
-        <c:axId val="225158848"/>
+        <c:axId val="21139392"/>
+        <c:axId val="21139968"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="225158272"/>
+        <c:axId val="21139392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4"/>
@@ -9596,13 +9595,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="225158848"/>
+        <c:crossAx val="21139968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="225158848"/>
+        <c:axId val="21139968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4"/>
@@ -9641,7 +9640,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="225158272"/>
+        <c:crossAx val="21139392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2"/>
@@ -9992,9 +9991,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q319"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -10013,16 +10010,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" s="3" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
-        <v>11</v>
+      <c r="A1" s="17" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B3" s="9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
@@ -10035,47 +10032,49 @@
       <c r="M3" s="6"/>
       <c r="N3" s="6"/>
       <c r="O3" s="6"/>
-      <c r="P3" s="7"/>
-      <c r="Q3" s="13"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="7"/>
     </row>
     <row r="4" spans="1:17" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="1"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B5" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D5" s="8" t="str">
         <f>_xll.tdmPyScript(D3,D7)</f>
-        <v>[pca_decomposition.xlsx]pca_decomposition!$D$5:5</v>
+        <v>[pca_decomposition.xlsx]pca_decomposition!$D$5:1</v>
       </c>
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
-      <c r="H5" s="7"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="7"/>
     </row>
     <row r="6" spans="1:17" ht="5.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="1"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B7" s="9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D7" s="8" t="str">
         <f>_xll.tdmGrid(B9:E14)</f>
-        <v>[pca_decomposition.xlsx]pca_decomposition!$D$7:5</v>
+        <v>[pca_decomposition.xlsx]pca_decomposition!$D$7:0</v>
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
-      <c r="H7" s="7"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="7"/>
     </row>
     <row r="8" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="1"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B9" s="10" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D9" s="4">
         <v>3</v>
@@ -10109,7 +10108,7 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B14" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D14" s="4">
         <v>0</v>
@@ -10119,44 +10118,44 @@
       <c r="B15" s="1"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B16" s="19"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="20"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="20"/>
-      <c r="H16" s="20"/>
-      <c r="I16" s="20"/>
-      <c r="J16" s="20"/>
-      <c r="K16" s="20"/>
-      <c r="L16" s="20"/>
-      <c r="M16" s="20"/>
-      <c r="N16" s="20"/>
-      <c r="O16" s="20"/>
-      <c r="P16" s="20"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="19"/>
+      <c r="J16" s="19"/>
+      <c r="K16" s="19"/>
+      <c r="L16" s="19"/>
+      <c r="M16" s="19"/>
+      <c r="N16" s="19"/>
+      <c r="O16" s="19"/>
+      <c r="P16" s="19"/>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B18" s="21" t="s">
-        <v>13</v>
+      <c r="B18" s="20" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="2:15" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D19" s="22" t="s">
+      <c r="D19" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="E19" s="22"/>
+      <c r="G19" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="E19" s="23"/>
-      <c r="G19" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="H19" s="23"/>
-      <c r="K19" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="L19" s="25"/>
-      <c r="N19" s="26" t="s">
+      <c r="H19" s="22"/>
+      <c r="K19" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="O19" s="27"/>
+      <c r="L19" s="24"/>
+      <c r="N19" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="O19" s="26"/>
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.2">
       <c r="D20" s="12">
@@ -10166,14 +10165,14 @@
       <c r="E20" s="12">
         <v>-1.3638951376004409</v>
       </c>
-      <c r="G20" s="14">
+      <c r="G20" s="13">
         <f t="array" ref="G20:H21">_xll.tdmLookup($D$5,$G$19)</f>
         <v>0.85065080835203988</v>
       </c>
-      <c r="H20" s="15">
+      <c r="H20" s="14">
         <v>-0.52573111211913348</v>
       </c>
-      <c r="I20" s="16">
+      <c r="I20" s="15">
         <f>G20/H20</f>
         <v>-1.6180339887498951</v>
       </c>
@@ -10202,13 +10201,13 @@
       <c r="E21" s="12">
         <v>1.262155215095718</v>
       </c>
-      <c r="G21" s="14">
+      <c r="G21" s="13">
         <v>0.52573111211913348</v>
       </c>
-      <c r="H21" s="15">
+      <c r="H21" s="14">
         <v>0.85065080835203988</v>
       </c>
-      <c r="I21" s="17">
+      <c r="I21" s="16">
         <f>G21/H21</f>
         <v>0.61803398874989479</v>
       </c>
@@ -10254,10 +10253,10 @@
       <c r="E23" s="12">
         <v>-1.1014456258232872</v>
       </c>
-      <c r="G23" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="H23" s="23"/>
+      <c r="G23" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="H23" s="22"/>
       <c r="K23" s="12">
         <v>2.3360065611018972</v>
       </c>
@@ -10279,14 +10278,14 @@
       <c r="E24" s="12">
         <v>0.51381735373193005</v>
       </c>
-      <c r="G24" s="14">
+      <c r="G24" s="13">
         <f t="array" ref="G24:H25">_xll.tdmLookup($D$5,$G$23)</f>
         <v>0.83462956668806398</v>
       </c>
-      <c r="H24" s="15">
+      <c r="H24" s="14">
         <v>0.55081166146886762</v>
       </c>
-      <c r="I24" s="16">
+      <c r="I24" s="15">
         <f>G24/H24</f>
         <v>1.5152721430449199</v>
       </c>
@@ -10311,13 +10310,13 @@
       <c r="E25" s="12">
         <v>1.3102299358020968</v>
       </c>
-      <c r="G25" s="14">
+      <c r="G25" s="13">
         <v>0.55081166146886762</v>
       </c>
-      <c r="H25" s="15">
+      <c r="H25" s="14">
         <v>-0.83462956668806398</v>
       </c>
-      <c r="I25" s="17">
+      <c r="I25" s="16">
         <f>G25/H25</f>
         <v>-0.65994745867267968</v>
       </c>

</xml_diff>

<commit_message>
Read inter process input argument from the text file
</commit_message>
<xml_diff>
--- a/examples/pca_decomposition/pca_decomposition.xlsx
+++ b/examples/pca_decomposition/pca_decomposition.xlsx
@@ -55,7 +55,7 @@
     <t>RESULT</t>
   </si>
   <si>
-    <t>D:\Users\Tandem Algorithms\My Development\GitHub\tandem-algorithms\examples\pca_decomposition\pca_decomposition.py</t>
+    <t>D:\Users\Tandem Algorithms\MyDevelopment\GitHub\tandem-algorithms\examples\pca_decomposition\pca_decomposition.py</t>
   </si>
 </sst>
 </file>
@@ -368,154 +368,154 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="300"/>
                 <c:pt idx="0">
-                  <c:v>-3.1016074093238863</c:v>
+                  <c:v>-3.298574878725764</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-2.9685794866286299</c:v>
+                  <c:v>-2.8273015821476974</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-2.41778135780703</c:v>
+                  <c:v>-2.8001715145991186</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-1.4437314527037302</c:v>
+                  <c:v>-1.5953471421287813</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-8.6752219445988987E-2</c:v>
+                  <c:v>-2.1362449557817492E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-1.1318578502408401</c:v>
+                  <c:v>-0.97150846431236304</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-1.3065842017830078</c:v>
+                  <c:v>-1.3978832248512061</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.92440787242906031</c:v>
+                  <c:v>-0.94505207925248624</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-2.2906759421687668</c:v>
+                  <c:v>-2.5250236186137709</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.1306014483965074E-2</c:v>
+                  <c:v>-0.1284643813395443</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.7268657872907642</c:v>
+                  <c:v>4.1649165765948473</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-0.94000394298800316</c:v>
+                  <c:v>-1.1529690614774375</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-2.7736927087609806</c:v>
+                  <c:v>-3.2715243295705934</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4.1647145192488161E-2</c:v>
+                  <c:v>1.2018548796580736E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-3.388202527547457</c:v>
+                  <c:v>-3.4201387193997577</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-0.48442749163235099</c:v>
+                  <c:v>-0.45915728708917769</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.6606670565513966</c:v>
+                  <c:v>2.5389534719981048</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.46630470569647697</c:v>
+                  <c:v>0.53435023312261143</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-2.7337637513964221</c:v>
+                  <c:v>-2.7565437172239053</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.81354133006853036</c:v>
+                  <c:v>0.83017472050027152</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.5742136862941565</c:v>
+                  <c:v>2.5445742996357965</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1.5551576637517777</c:v>
+                  <c:v>2.035817829460961</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1.0953793605083002</c:v>
+                  <c:v>1.11226451285018</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1.5465500076795724</c:v>
+                  <c:v>1.8181954267576632</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2.7428222956674717</c:v>
+                  <c:v>2.9420568788376582</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1.2097764377910976</c:v>
+                  <c:v>1.3829887153182421</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1.556170892214177</c:v>
+                  <c:v>1.4810593527901463</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>-0.21912385112196342</c:v>
+                  <c:v>-0.16202401401030964</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>-0.29456504009806828</c:v>
+                  <c:v>-0.26632535803392365</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1.2505410770896126</c:v>
+                  <c:v>1.2942057062086234</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>1.3102799351859984</c:v>
+                  <c:v>1.3596723098360501</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2.3825996446021298</c:v>
+                  <c:v>2.2820381706635873</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>-3.8767254050886851E-2</c:v>
+                  <c:v>-0.11343753707577428</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>2.3517011704896866</c:v>
+                  <c:v>2.6370529271427077</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>1.4359355713481932</c:v>
+                  <c:v>1.5692309550064412</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>-1.2594091332959976</c:v>
+                  <c:v>-1.3453346811645239</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>-1.0804247072314288</c:v>
+                  <c:v>-1.3929758311627096</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>-0.22776653847466866</c:v>
+                  <c:v>-0.36900841771634313</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>1.7667281518836884</c:v>
+                  <c:v>1.8166331877928579</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.46939049577543013</c:v>
+                  <c:v>0.51991896160788809</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>1.3285106574701482</c:v>
+                  <c:v>1.6032095266440509</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.19599315835367093</c:v>
+                  <c:v>-5.977184802549973E-2</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>-3.5797665830828085</c:v>
+                  <c:v>-3.5525413655823783</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>-1.7961057474280631</c:v>
+                  <c:v>-1.9832400171325459</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>1.0808271284076445</c:v>
+                  <c:v>1.3613946406106843</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>-0.10315859919307868</c:v>
+                  <c:v>0.10492523587787572</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>-0.94059211282138211</c:v>
+                  <c:v>-0.84850144592058085</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>-1.0132991765578467</c:v>
+                  <c:v>-0.97543054893021364</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>-1.1207180551482334</c:v>
+                  <c:v>-0.90054400694640813</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>-0.45379116930259467</c:v>
+                  <c:v>-0.42164425355533997</c:v>
                 </c:pt>
                 <c:pt idx="50">
                   <c:v>#N/A</c:v>
@@ -1277,154 +1277,154 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="300"/>
                 <c:pt idx="0">
-                  <c:v>-1.9168987987206692</c:v>
+                  <c:v>-2.6077524123467759</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-1.8346830210422072</c:v>
+                  <c:v>-2.2351781579460943</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-1.4942710564906152</c:v>
+                  <c:v>-2.2137299563141619</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.89227510839816637</c:v>
+                  <c:v>-1.2612326569418282</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-5.3615820217110761E-2</c:v>
+                  <c:v>-1.6888499250790032E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.69952662188222747</c:v>
+                  <c:v>-0.76804487833986868</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.80751344586554974</c:v>
+                  <c:v>-1.1051237233677751</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.57131548462913606</c:v>
+                  <c:v>-0.74712926947895342</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-1.4157155894719862</c:v>
+                  <c:v>-1.9962064451349621</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.3167841115887965E-2</c:v>
+                  <c:v>-0.10156001080934814</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.3033297280548282</c:v>
+                  <c:v>3.2926556616577125</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-0.58095438632550433</c:v>
+                  <c:v>-0.91150207649385073</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-1.7142363683620492</c:v>
+                  <c:v>-2.5863670755246053</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.5739351263359463E-2</c:v>
+                  <c:v>9.5014970917677039E-3</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-2.0940243227926301</c:v>
+                  <c:v>-2.7038570667586854</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-0.29939265491364819</c:v>
+                  <c:v>-0.36299570786640639</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.6443826736959015</c:v>
+                  <c:v>2.0072189611766373</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.28819215723443947</c:v>
+                  <c:v>0.42244095122734987</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-1.6895589155754065</c:v>
+                  <c:v>-2.1792391540636644</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.50279619323514857</c:v>
+                  <c:v>0.65631074316863414</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1.590951552434948</c:v>
+                  <c:v>2.0116626155942194</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.96114029406347878</c:v>
+                  <c:v>1.6094553105692191</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.6769816753692538</c:v>
+                  <c:v>0.87932230529604727</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.95582047004738657</c:v>
+                  <c:v>1.4374096949640176</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1.6951574038235109</c:v>
+                  <c:v>2.3259001857232584</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.74768295734367096</c:v>
+                  <c:v>1.0933485796789608</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.96176650369161043</c:v>
+                  <c:v>1.1708802261779294</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>-0.13542598773914516</c:v>
+                  <c:v>-0.12809122997890265</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>-0.18205120667808183</c:v>
+                  <c:v>-0.21054868251175549</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.77287688996928294</c:v>
+                  <c:v>1.0231594481014925</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.80979753472195626</c:v>
+                  <c:v>1.0749153426360201</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>1.472527561947536</c:v>
+                  <c:v>1.8041095816852442</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>-2.3959480653950118E-2</c:v>
+                  <c:v>-8.9680247329810808E-2</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>1.4534312547455375</c:v>
+                  <c:v>2.0847733900462542</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.88745698874818302</c:v>
+                  <c:v>1.2405859981653899</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>-0.77835765011897329</c:v>
+                  <c:v>-1.0635804519240808</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>-0.66773919135417725</c:v>
+                  <c:v>-1.1012440880100791</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>-0.14076746227725584</c:v>
+                  <c:v>-0.29172676893961835</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>1.0918980467454058</c:v>
+                  <c:v>1.4361746366194554</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.29009928038537974</c:v>
+                  <c:v>0.41103202934764144</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.82106474073302094</c:v>
+                  <c:v>1.2674484176689009</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.12113043342500901</c:v>
+                  <c:v>-4.7253794929504309E-2</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>-2.2124174201362496</c:v>
+                  <c:v>-2.8085305493013055</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>-1.1100543992995768</c:v>
+                  <c:v>-1.5678889002325509</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.6679879013188712</c:v>
+                  <c:v>1.0762769646690316</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>-6.375552053315009E-2</c:v>
+                  <c:v>8.2950682351126029E-2</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>-0.58131789527368982</c:v>
+                  <c:v>-0.67079929176380526</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>-0.62625333188502985</c:v>
+                  <c:v>-0.77114555848194843</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>-0.69264184988728728</c:v>
+                  <c:v>-0.71194254879128605</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>-0.28045836642356137</c:v>
+                  <c:v>-0.33333905088910581</c:v>
                 </c:pt>
                 <c:pt idx="50">
                   <c:v>#N/A</c:v>
@@ -2226,154 +2226,154 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="300"/>
                 <c:pt idx="0">
-                  <c:v>-3.1016074093238863</c:v>
+                  <c:v>-3.298574878725764</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-2.9685794866286299</c:v>
+                  <c:v>-2.8273015821476974</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-2.41778135780703</c:v>
+                  <c:v>-2.8001715145991186</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-1.4437314527037302</c:v>
+                  <c:v>-1.5953471421287813</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-8.6752219445988987E-2</c:v>
+                  <c:v>-2.1362449557817492E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-1.1318578502408401</c:v>
+                  <c:v>-0.97150846431236304</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-1.3065842017830078</c:v>
+                  <c:v>-1.3978832248512061</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.92440787242906031</c:v>
+                  <c:v>-0.94505207925248624</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-2.2906759421687668</c:v>
+                  <c:v>-2.5250236186137709</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.1306014483965074E-2</c:v>
+                  <c:v>-0.1284643813395443</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.7268657872907642</c:v>
+                  <c:v>4.1649165765948473</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-0.94000394298800316</c:v>
+                  <c:v>-1.1529690614774375</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-2.7736927087609806</c:v>
+                  <c:v>-3.2715243295705934</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4.1647145192488161E-2</c:v>
+                  <c:v>1.2018548796580736E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-3.388202527547457</c:v>
+                  <c:v>-3.4201387193997577</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-0.48442749163235099</c:v>
+                  <c:v>-0.45915728708917769</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.6606670565513966</c:v>
+                  <c:v>2.5389534719981048</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.46630470569647697</c:v>
+                  <c:v>0.53435023312261143</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-2.7337637513964221</c:v>
+                  <c:v>-2.7565437172239053</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.81354133006853036</c:v>
+                  <c:v>0.83017472050027152</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.5742136862941565</c:v>
+                  <c:v>2.5445742996357965</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1.5551576637517777</c:v>
+                  <c:v>2.035817829460961</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1.0953793605083002</c:v>
+                  <c:v>1.11226451285018</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1.5465500076795724</c:v>
+                  <c:v>1.8181954267576632</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2.7428222956674717</c:v>
+                  <c:v>2.9420568788376582</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1.2097764377910976</c:v>
+                  <c:v>1.3829887153182421</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1.556170892214177</c:v>
+                  <c:v>1.4810593527901463</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>-0.21912385112196342</c:v>
+                  <c:v>-0.16202401401030964</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>-0.29456504009806828</c:v>
+                  <c:v>-0.26632535803392365</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1.2505410770896126</c:v>
+                  <c:v>1.2942057062086234</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>1.3102799351859984</c:v>
+                  <c:v>1.3596723098360501</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2.3825996446021298</c:v>
+                  <c:v>2.2820381706635873</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>-3.8767254050886851E-2</c:v>
+                  <c:v>-0.11343753707577428</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>2.3517011704896866</c:v>
+                  <c:v>2.6370529271427077</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>1.4359355713481932</c:v>
+                  <c:v>1.5692309550064412</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>-1.2594091332959976</c:v>
+                  <c:v>-1.3453346811645239</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>-1.0804247072314288</c:v>
+                  <c:v>-1.3929758311627096</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>-0.22776653847466866</c:v>
+                  <c:v>-0.36900841771634313</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>1.7667281518836884</c:v>
+                  <c:v>1.8166331877928579</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.46939049577543013</c:v>
+                  <c:v>0.51991896160788809</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>1.3285106574701482</c:v>
+                  <c:v>1.6032095266440509</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.19599315835367093</c:v>
+                  <c:v>-5.977184802549973E-2</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>-3.5797665830828085</c:v>
+                  <c:v>-3.5525413655823783</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>-1.7961057474280631</c:v>
+                  <c:v>-1.9832400171325459</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>1.0808271284076445</c:v>
+                  <c:v>1.3613946406106843</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>-0.10315859919307868</c:v>
+                  <c:v>0.10492523587787572</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>-0.94059211282138211</c:v>
+                  <c:v>-0.84850144592058085</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>-1.0132991765578467</c:v>
+                  <c:v>-0.97543054893021364</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>-1.1207180551482334</c:v>
+                  <c:v>-0.90054400694640813</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>-0.45379116930259467</c:v>
+                  <c:v>-0.42164425355533997</c:v>
                 </c:pt>
                 <c:pt idx="50">
                   <c:v>#N/A</c:v>
@@ -3135,154 +3135,154 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="300"/>
                 <c:pt idx="0">
-                  <c:v>-1.3638951376004409</c:v>
+                  <c:v>-1.4589552635380152</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.262155215095718</c:v>
+                  <c:v>0.90884738915417407</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-2.8448358700263783</c:v>
+                  <c:v>-2.73690837979166</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-1.1014456258232872</c:v>
+                  <c:v>-1.0980237762708427</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.51381735373193005</c:v>
+                  <c:v>0.4547646281458928</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.3102299358020968</c:v>
+                  <c:v>1.0908230921970343</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.639362708654165</c:v>
+                  <c:v>-0.67278641135462713</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.11018890537115889</c:v>
+                  <c:v>-0.1687943763747603</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-1.6992373369234071</c:v>
+                  <c:v>-1.6987485686757164</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-1.1671634409526259</c:v>
+                  <c:v>-1.0463050536852585</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.2066084112744391</c:v>
+                  <c:v>3.1606547474661997</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-1.6066012192659476</c:v>
+                  <c:v>-1.513498134033016</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-3.7241202985863722</c:v>
+                  <c:v>-3.5532555056976376</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-0.23294236732727963</c:v>
+                  <c:v>-0.20599529207929601</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-6.3420444458172742E-2</c:v>
+                  <c:v>-0.31300884695931019</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.22321509390525715</c:v>
+                  <c:v>0.16379811893780888</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-1.0930107205938138</c:v>
+                  <c:v>-0.78025515359969366</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.50426111843013266</c:v>
+                  <c:v>0.48798277580607641</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-2.7910831943309677E-2</c:v>
+                  <c:v>-0.23166712173813697</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>8.5024066832616763E-2</c:v>
+                  <c:v>0.13782171941336896</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-0.37146497211188234</c:v>
+                  <c:v>-0.13896298888945968</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>3.6570455858568018</c:v>
+                  <c:v>3.4009413178641887</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>7.1577880140467232E-2</c:v>
+                  <c:v>0.14704961171049302</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2.0302857158818362</c:v>
+                  <c:v>1.9397356687235576</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1.4011575673439829</c:v>
+                  <c:v>1.4652949472004522</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1.2823690590529375</c:v>
+                  <c:v>1.2427809381294084</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>-0.66982704655353886</c:v>
+                  <c:v>-0.48378161867430658</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.4565140988690724</c:v>
+                  <c:v>0.39331183477641812</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.23595467535661346</c:v>
+                  <c:v>0.18958522078003032</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.27158092769382552</c:v>
+                  <c:v>0.33834506565874178</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.31290728623540981</c:v>
+                  <c:v>0.3799639886949574</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>-0.91313632028722236</c:v>
+                  <c:v>-0.63977370026823366</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>-0.57920707846201458</c:v>
+                  <c:v>-0.52295984203446566</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>2.0929806024918185</c:v>
+                  <c:v>2.0568754641042482</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.95924376017938107</c:v>
+                  <c:v>0.96976137727618472</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>-0.60010765142012623</c:v>
+                  <c:v>-0.6339766919300811</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>-2.3742265048969529</c:v>
+                  <c:v>-2.2133082479746728</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>-1.0871517321178621</c:v>
+                  <c:v>-0.99329207448549706</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.29194748441746643</c:v>
+                  <c:v>0.39564232845712016</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.36771787435711811</c:v>
+                  <c:v>0.36562325867027584</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>2.0659763277375434</c:v>
+                  <c:v>1.9553011785564176</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>-2.0019061260076834</c:v>
+                  <c:v>-1.7825605268413125</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.40763698223498301</c:v>
+                  <c:v>9.5443304528013861E-2</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>-1.3587044069720016</c:v>
+                  <c:v>-1.3556298003331999</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>2.1252043484416792</c:v>
+                  <c:v>1.9897588998079581</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>1.6256220173556069</c:v>
+                  <c:v>1.4517371631166123</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.76836405840685229</c:v>
+                  <c:v>0.6187743870433039</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.35020677101754616</c:v>
+                  <c:v>0.23784496028199742</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>1.7753704731850142</c:v>
+                  <c:v>1.5092824976949624</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.27507727074108163</c:v>
+                  <c:v>0.21267696037101397</c:v>
                 </c:pt>
                 <c:pt idx="50">
                   <c:v>#N/A</c:v>
@@ -4072,154 +4072,154 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="300"/>
                 <c:pt idx="0">
-                  <c:v>-3.1016074093238863</c:v>
+                  <c:v>-3.298574878725764</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-2.9685794866286299</c:v>
+                  <c:v>-2.8273015821476974</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-2.41778135780703</c:v>
+                  <c:v>-2.8001715145991186</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-1.4437314527037302</c:v>
+                  <c:v>-1.5953471421287813</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-8.6752219445988987E-2</c:v>
+                  <c:v>-2.1362449557817492E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-1.1318578502408401</c:v>
+                  <c:v>-0.97150846431236304</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-1.3065842017830078</c:v>
+                  <c:v>-1.3978832248512061</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.92440787242906031</c:v>
+                  <c:v>-0.94505207925248624</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-2.2906759421687668</c:v>
+                  <c:v>-2.5250236186137709</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.1306014483965074E-2</c:v>
+                  <c:v>-0.1284643813395443</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.7268657872907642</c:v>
+                  <c:v>4.1649165765948473</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-0.94000394298800316</c:v>
+                  <c:v>-1.1529690614774375</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-2.7736927087609806</c:v>
+                  <c:v>-3.2715243295705934</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4.1647145192488161E-2</c:v>
+                  <c:v>1.2018548796580736E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-3.388202527547457</c:v>
+                  <c:v>-3.4201387193997577</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-0.48442749163235099</c:v>
+                  <c:v>-0.45915728708917769</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.6606670565513966</c:v>
+                  <c:v>2.5389534719981048</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.46630470569647697</c:v>
+                  <c:v>0.53435023312261143</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-2.7337637513964221</c:v>
+                  <c:v>-2.7565437172239053</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.81354133006853036</c:v>
+                  <c:v>0.83017472050027152</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.5742136862941565</c:v>
+                  <c:v>2.5445742996357965</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1.5551576637517777</c:v>
+                  <c:v>2.035817829460961</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1.0953793605083002</c:v>
+                  <c:v>1.11226451285018</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1.5465500076795724</c:v>
+                  <c:v>1.8181954267576632</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2.7428222956674717</c:v>
+                  <c:v>2.9420568788376582</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1.2097764377910976</c:v>
+                  <c:v>1.3829887153182421</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1.556170892214177</c:v>
+                  <c:v>1.4810593527901463</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>-0.21912385112196342</c:v>
+                  <c:v>-0.16202401401030964</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>-0.29456504009806828</c:v>
+                  <c:v>-0.26632535803392365</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1.2505410770896126</c:v>
+                  <c:v>1.2942057062086234</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>1.3102799351859984</c:v>
+                  <c:v>1.3596723098360501</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2.3825996446021298</c:v>
+                  <c:v>2.2820381706635873</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>-3.8767254050886851E-2</c:v>
+                  <c:v>-0.11343753707577428</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>2.3517011704896866</c:v>
+                  <c:v>2.6370529271427077</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>1.4359355713481932</c:v>
+                  <c:v>1.5692309550064412</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>-1.2594091332959976</c:v>
+                  <c:v>-1.3453346811645239</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>-1.0804247072314288</c:v>
+                  <c:v>-1.3929758311627096</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>-0.22776653847466866</c:v>
+                  <c:v>-0.36900841771634313</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>1.7667281518836884</c:v>
+                  <c:v>1.8166331877928579</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.46939049577543013</c:v>
+                  <c:v>0.51991896160788809</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>1.3285106574701482</c:v>
+                  <c:v>1.6032095266440509</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.19599315835367093</c:v>
+                  <c:v>-5.977184802549973E-2</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>-3.5797665830828085</c:v>
+                  <c:v>-3.5525413655823783</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>-1.7961057474280631</c:v>
+                  <c:v>-1.9832400171325459</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>1.0808271284076445</c:v>
+                  <c:v>1.3613946406106843</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>-0.10315859919307868</c:v>
+                  <c:v>0.10492523587787572</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>-0.94059211282138211</c:v>
+                  <c:v>-0.84850144592058085</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>-1.0132991765578467</c:v>
+                  <c:v>-0.97543054893021364</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>-1.1207180551482334</c:v>
+                  <c:v>-0.90054400694640813</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>-0.45379116930259467</c:v>
+                  <c:v>-0.42164425355533997</c:v>
                 </c:pt>
                 <c:pt idx="50">
                   <c:v>#N/A</c:v>
@@ -4981,154 +4981,154 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="300"/>
                 <c:pt idx="0">
-                  <c:v>5.0185062080445562</c:v>
+                  <c:v>5.2155048246935518</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.803262507670838</c:v>
+                  <c:v>4.4703563158921886</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.9120524142976461</c:v>
+                  <c:v>4.4274599126283238</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.3360065611018972</c:v>
+                  <c:v>2.5224653138836564</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.14036803966309977</c:v>
+                  <c:v>3.3776998501580065E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.8313844721230679</c:v>
+                  <c:v>1.5360897566797374</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.114097647648558</c:v>
+                  <c:v>2.2102474467355502</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.4957233570581967</c:v>
+                  <c:v>1.4942585389579068</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.7063915316407536</c:v>
+                  <c:v>3.9924128902699243</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-3.4473855599853047E-2</c:v>
+                  <c:v>0.20312002161869627</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-6.0301955153455937</c:v>
+                  <c:v>-6.585311323315425</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.5209583293135078</c:v>
+                  <c:v>1.8230041529877015</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4.4879290771230309</c:v>
+                  <c:v>5.1727341510492106</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-6.7386496455847641E-2</c:v>
+                  <c:v>-1.9002994183535408E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>5.4822268503400879</c:v>
+                  <c:v>5.4077141335173708</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.7838201465459993</c:v>
+                  <c:v>0.72599141573281278</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-4.3050497302472985</c:v>
+                  <c:v>-4.0144379223532747</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-0.75449686293091656</c:v>
+                  <c:v>-0.84488190245469974</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>4.4233226669718295</c:v>
+                  <c:v>4.3584783081273288</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-1.3163375233036791</c:v>
+                  <c:v>-1.3126214863372683</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-4.1651652387291049</c:v>
+                  <c:v>-4.0233252311884389</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>-2.5162979578152571</c:v>
+                  <c:v>-3.2189106211384382</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>-1.7723610358775543</c:v>
+                  <c:v>-1.7586446105920945</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>-2.5023704777269593</c:v>
+                  <c:v>-2.8748193899280352</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>-4.4379796994909837</c:v>
+                  <c:v>-4.6518003714465168</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>-1.957459395134769</c:v>
+                  <c:v>-2.1866971593579216</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>-2.517937395905788</c:v>
+                  <c:v>-2.3417604523558588</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.35454983886110863</c:v>
+                  <c:v>0.25618245995780531</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.47661624677615022</c:v>
+                  <c:v>0.42109736502351097</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>-2.0234179670588959</c:v>
+                  <c:v>-2.046318896202985</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>-2.120077469907955</c:v>
+                  <c:v>-2.1498306852720401</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>-3.8551272065496667</c:v>
+                  <c:v>-3.6082191633704883</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>6.2726734704836987E-2</c:v>
+                  <c:v>0.17936049465962162</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>-3.8051324252352248</c:v>
+                  <c:v>-4.1695467800925083</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>-2.3233925600963765</c:v>
+                  <c:v>-2.4811719963307799</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>2.0377667834149715</c:v>
+                  <c:v>2.1271609038481616</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>1.7481638985856065</c:v>
+                  <c:v>2.2024881760201582</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.36853400075192461</c:v>
+                  <c:v>0.58345353787923671</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>-2.8586261986290946</c:v>
+                  <c:v>-2.8723492732389109</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>-0.75948977616081004</c:v>
+                  <c:v>-0.82206405869528287</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>-2.1495753982031696</c:v>
+                  <c:v>-2.5348968353378019</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>-0.31712359177867999</c:v>
+                  <c:v>9.4507589859008617E-2</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>5.7921840032190595</c:v>
+                  <c:v>5.617061098602611</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>2.9061601467276406</c:v>
+                  <c:v>3.1357778004651018</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>-1.7488150297265161</c:v>
+                  <c:v>-2.1525539293380631</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.1669141197262288</c:v>
+                  <c:v>-0.16590136470225206</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>1.5219100080950723</c:v>
+                  <c:v>1.3415985835276105</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>1.639552508442877</c:v>
+                  <c:v>1.5422911169638969</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>1.8133599050355211</c:v>
+                  <c:v>1.4238850975825721</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.73424953572615625</c:v>
+                  <c:v>0.66667810177821163</c:v>
                 </c:pt>
                 <c:pt idx="50">
                   <c:v>#N/A</c:v>
@@ -5905,154 +5905,154 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="300"/>
                 <c:pt idx="0">
-                  <c:v>-3.1016074093238863</c:v>
+                  <c:v>-3.298574878725764</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-2.9685794866286299</c:v>
+                  <c:v>-2.8273015821476974</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-2.41778135780703</c:v>
+                  <c:v>-2.8001715145991186</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-1.4437314527037302</c:v>
+                  <c:v>-1.5953471421287813</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-8.6752219445988987E-2</c:v>
+                  <c:v>-2.1362449557817492E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-1.1318578502408401</c:v>
+                  <c:v>-0.97150846431236304</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-1.3065842017830078</c:v>
+                  <c:v>-1.3978832248512061</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.92440787242906031</c:v>
+                  <c:v>-0.94505207925248624</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-2.2906759421687668</c:v>
+                  <c:v>-2.5250236186137709</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.1306014483965074E-2</c:v>
+                  <c:v>-0.1284643813395443</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.7268657872907642</c:v>
+                  <c:v>4.1649165765948473</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-0.94000394298800316</c:v>
+                  <c:v>-1.1529690614774375</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-2.7736927087609806</c:v>
+                  <c:v>-3.2715243295705934</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4.1647145192488161E-2</c:v>
+                  <c:v>1.2018548796580736E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-3.388202527547457</c:v>
+                  <c:v>-3.4201387193997577</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-0.48442749163235099</c:v>
+                  <c:v>-0.45915728708917769</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.6606670565513966</c:v>
+                  <c:v>2.5389534719981048</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.46630470569647697</c:v>
+                  <c:v>0.53435023312261143</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-2.7337637513964221</c:v>
+                  <c:v>-2.7565437172239053</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.81354133006853036</c:v>
+                  <c:v>0.83017472050027152</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.5742136862941565</c:v>
+                  <c:v>2.5445742996357965</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1.5551576637517777</c:v>
+                  <c:v>2.035817829460961</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1.0953793605083002</c:v>
+                  <c:v>1.11226451285018</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1.5465500076795724</c:v>
+                  <c:v>1.8181954267576632</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2.7428222956674717</c:v>
+                  <c:v>2.9420568788376582</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1.2097764377910976</c:v>
+                  <c:v>1.3829887153182421</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1.556170892214177</c:v>
+                  <c:v>1.4810593527901463</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>-0.21912385112196342</c:v>
+                  <c:v>-0.16202401401030964</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>-0.29456504009806828</c:v>
+                  <c:v>-0.26632535803392365</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1.2505410770896126</c:v>
+                  <c:v>1.2942057062086234</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>1.3102799351859984</c:v>
+                  <c:v>1.3596723098360501</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2.3825996446021298</c:v>
+                  <c:v>2.2820381706635873</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>-3.8767254050886851E-2</c:v>
+                  <c:v>-0.11343753707577428</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>2.3517011704896866</c:v>
+                  <c:v>2.6370529271427077</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>1.4359355713481932</c:v>
+                  <c:v>1.5692309550064412</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>-1.2594091332959976</c:v>
+                  <c:v>-1.3453346811645239</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>-1.0804247072314288</c:v>
+                  <c:v>-1.3929758311627096</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>-0.22776653847466866</c:v>
+                  <c:v>-0.36900841771634313</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>1.7667281518836884</c:v>
+                  <c:v>1.8166331877928579</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.46939049577543013</c:v>
+                  <c:v>0.51991896160788809</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>1.3285106574701482</c:v>
+                  <c:v>1.6032095266440509</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.19599315835367093</c:v>
+                  <c:v>-5.977184802549973E-2</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>-3.5797665830828085</c:v>
+                  <c:v>-3.5525413655823783</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>-1.7961057474280631</c:v>
+                  <c:v>-1.9832400171325459</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>1.0808271284076445</c:v>
+                  <c:v>1.3613946406106843</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>-0.10315859919307868</c:v>
+                  <c:v>0.10492523587787572</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>-0.94059211282138211</c:v>
+                  <c:v>-0.84850144592058085</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>-1.0132991765578467</c:v>
+                  <c:v>-0.97543054893021364</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>-1.1207180551482334</c:v>
+                  <c:v>-0.90054400694640813</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>-0.45379116930259467</c:v>
+                  <c:v>-0.42164425355533997</c:v>
                 </c:pt>
                 <c:pt idx="50">
                   <c:v>#N/A</c:v>
@@ -6814,154 +6814,154 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="300"/>
                 <c:pt idx="0">
-                  <c:v>4.6997793060102069</c:v>
+                  <c:v>5.4390118808374499</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.4982058005029524</c:v>
+                  <c:v>4.6619305189010118</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.6635967394583147</c:v>
+                  <c:v>4.6171958182651895</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.1876460523197365</c:v>
+                  <c:v>2.6305639190008239</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.1314532214738269</c:v>
+                  <c:v>3.5224489732864385E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.7150726703566537</c:v>
+                  <c:v>1.6019178809032553</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.9798306435043742</c:v>
+                  <c:v>2.3049661588783299</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.400729497903177</c:v>
+                  <c:v>1.558294013640837</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.4709974439115081</c:v>
+                  <c:v>4.1635051396319236</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-3.2284410226863861E-2</c:v>
+                  <c:v>0.21182459760929506</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-5.6472159083488691</c:v>
+                  <c:v>-6.8675205431586424</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.4243617891621063</c:v>
+                  <c:v>1.9011278064532742</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4.2028992949523198</c:v>
+                  <c:v>5.3944082978819559</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-6.3106758947524461E-2</c:v>
+                  <c:v>-1.9817355099811845E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>5.1340489049870497</c:v>
+                  <c:v>5.6394581941742858</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.73403948339562752</c:v>
+                  <c:v>0.75710330414444238</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-4.0316346727096537</c:v>
+                  <c:v>-4.1864740400938665</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-0.70657853071263133</c:v>
+                  <c:v>-0.88108876509872025</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>4.1423960581569759</c:v>
+                  <c:v>4.5452580521138204</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-1.2327365146685565</c:v>
+                  <c:v>-1.3688730236483682</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-3.9006342890865096</c:v>
+                  <c:v>-4.1957422087501905</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>-2.3564870859258868</c:v>
+                  <c:v>-3.3568549354672528</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>-1.659797831044586</c:v>
+                  <c:v>-1.8340101778629228</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>-2.3434441444627629</c:v>
+                  <c:v>-2.998017899062952</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>-4.1561222179474369</c:v>
+                  <c:v>-4.8511502410638254</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>-1.8331405354969657</c:v>
+                  <c:v>-2.2804066393017024</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>-2.3580224027895009</c:v>
+                  <c:v>-2.4421150685422246</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.33203226748183345</c:v>
+                  <c:v>0.26716099212017091</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.44634619957551269</c:v>
+                  <c:v>0.43914321783544608</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>-1.8949100578472795</c:v>
+                  <c:v>-2.1340125572761166</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>-1.9854306853780466</c:v>
+                  <c:v>-2.2419602765242548</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>-3.6102868694943338</c:v>
+                  <c:v>-3.762847041252726</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>5.8742940125654168E-2</c:v>
+                  <c:v>0.18704687162548719</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>-3.5634672724091541</c:v>
+                  <c:v>-4.3482299867229424</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>-2.1758331704712082</c:v>
+                  <c:v>-2.5875010032681196</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>1.9083475763797715</c:v>
+                  <c:v>2.2183189964094949</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>1.6371374615252472</c:v>
+                  <c:v>2.2968743696793563</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.34512829086843438</c:v>
+                  <c:v>0.60845705854145615</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>-2.6770739528825871</c:v>
+                  <c:v>-2.9954419271348671</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>-0.71125434245855346</c:v>
+                  <c:v>-0.85729307753364292</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>-2.0130551910028069</c:v>
+                  <c:v>-2.6435281851953154</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>-0.29698297308070926</c:v>
+                  <c:v>9.8557650956187834E-2</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>5.4243205819484777</c:v>
+                  <c:v>5.857776586849301</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>2.7215890050406188</c:v>
+                  <c:v>3.2701595120081492</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>-1.6377472391233383</c:v>
+                  <c:v>-2.2448002234378097</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.15631335167280827</c:v>
+                  <c:v>-0.17301095943588057</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>1.4252530265260046</c:v>
+                  <c:v>1.3990919154312385</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>1.535424014808461</c:v>
+                  <c:v>1.6083849964360031</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>1.6981928491735983</c:v>
+                  <c:v>1.4849047643540521</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.68761711760400268</c:v>
+                  <c:v>0.69524815682227059</c:v>
                 </c:pt>
                 <c:pt idx="50">
                   <c:v>#N/A</c:v>
@@ -7738,154 +7738,154 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="300"/>
                 <c:pt idx="0">
-                  <c:v>-3.1016074093238863</c:v>
+                  <c:v>-3.298574878725764</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-2.9685794866286299</c:v>
+                  <c:v>-2.8273015821476974</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-2.41778135780703</c:v>
+                  <c:v>-2.8001715145991186</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-1.4437314527037302</c:v>
+                  <c:v>-1.5953471421287813</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-8.6752219445988987E-2</c:v>
+                  <c:v>-2.1362449557817492E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-1.1318578502408401</c:v>
+                  <c:v>-0.97150846431236304</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-1.3065842017830078</c:v>
+                  <c:v>-1.3978832248512061</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.92440787242906031</c:v>
+                  <c:v>-0.94505207925248624</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-2.2906759421687668</c:v>
+                  <c:v>-2.5250236186137709</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.1306014483965074E-2</c:v>
+                  <c:v>-0.1284643813395443</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.7268657872907642</c:v>
+                  <c:v>4.1649165765948473</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-0.94000394298800316</c:v>
+                  <c:v>-1.1529690614774375</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-2.7736927087609806</c:v>
+                  <c:v>-3.2715243295705934</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4.1647145192488161E-2</c:v>
+                  <c:v>1.2018548796580736E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-3.388202527547457</c:v>
+                  <c:v>-3.4201387193997577</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-0.48442749163235099</c:v>
+                  <c:v>-0.45915728708917769</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.6606670565513966</c:v>
+                  <c:v>2.5389534719981048</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.46630470569647697</c:v>
+                  <c:v>0.53435023312261143</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-2.7337637513964221</c:v>
+                  <c:v>-2.7565437172239053</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.81354133006853036</c:v>
+                  <c:v>0.83017472050027152</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.5742136862941565</c:v>
+                  <c:v>2.5445742996357965</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1.5551576637517777</c:v>
+                  <c:v>2.035817829460961</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1.0953793605083002</c:v>
+                  <c:v>1.11226451285018</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1.5465500076795724</c:v>
+                  <c:v>1.8181954267576632</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2.7428222956674717</c:v>
+                  <c:v>2.9420568788376582</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1.2097764377910976</c:v>
+                  <c:v>1.3829887153182421</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1.556170892214177</c:v>
+                  <c:v>1.4810593527901463</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>-0.21912385112196342</c:v>
+                  <c:v>-0.16202401401030964</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>-0.29456504009806828</c:v>
+                  <c:v>-0.26632535803392365</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1.2505410770896126</c:v>
+                  <c:v>1.2942057062086234</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>1.3102799351859984</c:v>
+                  <c:v>1.3596723098360501</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2.3825996446021298</c:v>
+                  <c:v>2.2820381706635873</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>-3.8767254050886851E-2</c:v>
+                  <c:v>-0.11343753707577428</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>2.3517011704896866</c:v>
+                  <c:v>2.6370529271427077</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>1.4359355713481932</c:v>
+                  <c:v>1.5692309550064412</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>-1.2594091332959976</c:v>
+                  <c:v>-1.3453346811645239</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>-1.0804247072314288</c:v>
+                  <c:v>-1.3929758311627096</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>-0.22776653847466866</c:v>
+                  <c:v>-0.36900841771634313</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>1.7667281518836884</c:v>
+                  <c:v>1.8166331877928579</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.46939049577543013</c:v>
+                  <c:v>0.51991896160788809</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>1.3285106574701482</c:v>
+                  <c:v>1.6032095266440509</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.19599315835367093</c:v>
+                  <c:v>-5.977184802549973E-2</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>-3.5797665830828085</c:v>
+                  <c:v>-3.5525413655823783</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>-1.7961057474280631</c:v>
+                  <c:v>-1.9832400171325459</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>1.0808271284076445</c:v>
+                  <c:v>1.3613946406106843</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>-0.10315859919307868</c:v>
+                  <c:v>0.10492523587787572</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>-0.94059211282138211</c:v>
+                  <c:v>-0.84850144592058085</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>-1.0132991765578467</c:v>
+                  <c:v>-0.97543054893021364</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>-1.1207180551482334</c:v>
+                  <c:v>-0.90054400694640813</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>-0.45379116930259467</c:v>
+                  <c:v>-0.42164425355533997</c:v>
                 </c:pt>
                 <c:pt idx="50">
                   <c:v>#N/A</c:v>
@@ -8647,154 +8647,154 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="300"/>
                 <c:pt idx="0">
-                  <c:v>-2.0468979275836525</c:v>
+                  <c:v>-2.00047296621926</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-1.9591064880684124</c:v>
+                  <c:v>-1.7146618131707518</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-1.5956086627109303</c:v>
+                  <c:v>-1.6982083541170649</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.9527869032176427</c:v>
+                  <c:v>-0.96752353573875383</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-5.7251906757595054E-2</c:v>
+                  <c:v>-1.2955595796310971E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.74696671184516483</c:v>
+                  <c:v>-0.58918669145410874</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.86227692350856777</c:v>
+                  <c:v>-0.84776841637940747</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.61006062618657697</c:v>
+                  <c:v>-0.57314179781306596</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-1.5117257666769237</c:v>
+                  <c:v>-1.5313405557897382</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.4060850113136056E-2</c:v>
+                  <c:v>-7.7909258222179617E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.4595356051366952</c:v>
+                  <c:v>2.52587960690922</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-0.62035321331723114</c:v>
+                  <c:v>-0.69923634392795653</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-1.8304914542857502</c:v>
+                  <c:v>-1.9840677323543832</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.748492763075467E-2</c:v>
+                  <c:v>7.2888392244212091E-3</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-2.2360356475232943</c:v>
+                  <c:v>-2.0741972822887655</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-0.31969669201395085</c:v>
+                  <c:v>-0.27846320724400336</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.755900462345213</c:v>
+                  <c:v>1.5397885359457997</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.30773660549150178</c:v>
+                  <c:v>0.32406516000257635</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-1.8041404403455601</c:v>
+                  <c:v>-1.6717495855780526</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.53689453330391834</c:v>
+                  <c:v>0.50347260458157805</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1.6988457803502592</c:v>
+                  <c:v>1.5431973758692166</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1.0263223480283274</c:v>
+                  <c:v>1.2346539586686796</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.72289282524995779</c:v>
+                  <c:v>0.67455042588008685</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1.0206417472783471</c:v>
+                  <c:v>1.1026734066250035</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1.8101186036165131</c:v>
+                  <c:v>1.784256979931804</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.79838888568232202</c:v>
+                  <c:v>0.83873540522723999</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1.0269910255771426</c:v>
+                  <c:v>0.89821189621362041</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>-0.14461022868251036</c:v>
+                  <c:v>-9.8262028852643193E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>-0.19439744962653616</c:v>
+                  <c:v>-0.16151723048692493</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.8252914057910854</c:v>
+                  <c:v>0.7848915435253645</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.86471591337580311</c:v>
+                  <c:v>0.82459480192083567</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>1.5723905804896054</c:v>
+                  <c:v>1.3839781833470082</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>-2.5584350790600924E-2</c:v>
+                  <c:v>-6.8795990577071212E-2</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>1.5519992110222349</c:v>
+                  <c:v>1.5992825038660994</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.94764203112894241</c:v>
+                  <c:v>0.95168496052376683</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>-0.83114385694785564</c:v>
+                  <c:v>-0.8158995199849719</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>-0.71302353982455535</c:v>
+                  <c:v>-0.84479224977129197</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>-0.1503139482370307</c:v>
+                  <c:v>-0.22379099795789728</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>1.1659477540011203</c:v>
+                  <c:v>1.1017259620676512</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.30977306481210432</c:v>
+                  <c:v>0.31531308688167564</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.87674723221699513</c:v>
+                  <c:v>0.97229180332432819</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.12934518677273721</c:v>
+                  <c:v>-3.6249583687537446E-2</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>-2.3624578591468817</c:v>
+                  <c:v>-2.1544949635851638</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>-1.1853354235225442</c:v>
+                  <c:v>-1.2027673118430131</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.71328911665711503</c:v>
+                  <c:v>0.82563933669121936</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>-6.8079255377705816E-2</c:v>
+                  <c:v>6.3633570728263644E-2</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>-0.62074137450403755</c:v>
+                  <c:v>-0.51458713740576989</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>-0.66872421644446989</c:v>
+                  <c:v>-0.59156530177453459</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>-0.73961503238366466</c:v>
+                  <c:v>-0.54614917260358875</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>-0.29947832894935106</c:v>
+                  <c:v>-0.25571283406032463</c:v>
                 </c:pt>
                 <c:pt idx="50">
                   <c:v>#N/A</c:v>
@@ -9559,11 +9559,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="21139392"/>
-        <c:axId val="21139968"/>
+        <c:axId val="1072629440"/>
+        <c:axId val="1072630016"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="21139392"/>
+        <c:axId val="1072629440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4"/>
@@ -9595,13 +9595,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="21139968"/>
+        <c:crossAx val="1072630016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="21139968"/>
+        <c:axId val="1072630016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4"/>
@@ -9640,7 +9640,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="21139392"/>
+        <c:crossAx val="1072629440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2"/>
@@ -9991,7 +9991,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q319"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -10044,7 +10046,7 @@
       </c>
       <c r="D5" s="8" t="str">
         <f>_xll.tdmPyScript(D3,D7)</f>
-        <v>[pca_decomposition.xlsx]pca_decomposition!$D$5:1</v>
+        <v>[pca_decomposition.xlsx]pca_decomposition!$D$5:9</v>
       </c>
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
@@ -10061,7 +10063,7 @@
       </c>
       <c r="D7" s="8" t="str">
         <f>_xll.tdmGrid(B9:E14)</f>
-        <v>[pca_decomposition.xlsx]pca_decomposition!$D$7:0</v>
+        <v>[pca_decomposition.xlsx]pca_decomposition!$D$7:8</v>
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
@@ -10086,7 +10088,7 @@
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B10" s="1"/>
       <c r="D10" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E10" s="4">
         <v>2</v>
@@ -10160,1102 +10162,1102 @@
     <row r="20" spans="2:15" x14ac:dyDescent="0.2">
       <c r="D20" s="12">
         <f t="array" ref="D20:E319">_xll.tdmLookup(D5,D19)</f>
-        <v>-3.1016074093238863</v>
+        <v>-3.298574878725764</v>
       </c>
       <c r="E20" s="12">
-        <v>-1.3638951376004409</v>
+        <v>-1.4589552635380152</v>
       </c>
       <c r="G20" s="13">
         <f t="array" ref="G20:H21">_xll.tdmLookup($D$5,$G$19)</f>
-        <v>0.85065080835203988</v>
+        <v>0.70710678118654746</v>
       </c>
       <c r="H20" s="14">
-        <v>-0.52573111211913348</v>
+        <v>-0.44721359549995793</v>
       </c>
       <c r="I20" s="15">
         <f>G20/H20</f>
-        <v>-1.6180339887498951</v>
+        <v>-1.5811388300841895</v>
       </c>
       <c r="K20" s="12">
         <f t="array" ref="K20:K319">$D$20:$D$135*$I$20</f>
-        <v>5.0185062080445562</v>
+        <v>5.2155048246935518</v>
       </c>
       <c r="L20" s="12">
         <f t="array" ref="L20:L319">$D$20:$D$135*$I$21</f>
-        <v>-1.9168987987206692</v>
+        <v>-2.6077524123467759</v>
       </c>
       <c r="M20" s="11"/>
       <c r="N20" s="12">
         <f t="array" ref="N20:N319">-$D$20:$D$135*$I$24</f>
-        <v>4.6997793060102069</v>
+        <v>5.4390118808374499</v>
       </c>
       <c r="O20" s="12">
         <f t="array" ref="O20:O319">-$D$20:$D$135*$I$25</f>
-        <v>-2.0468979275836525</v>
+        <v>-2.00047296621926</v>
       </c>
     </row>
     <row r="21" spans="2:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D21" s="12">
-        <v>-2.9685794866286299</v>
+        <v>-2.8273015821476974</v>
       </c>
       <c r="E21" s="12">
-        <v>1.262155215095718</v>
+        <v>0.90884738915417407</v>
       </c>
       <c r="G21" s="13">
-        <v>0.52573111211913348</v>
+        <v>0.70710678118654746</v>
       </c>
       <c r="H21" s="14">
-        <v>0.85065080835203988</v>
+        <v>0.89442719099991586</v>
       </c>
       <c r="I21" s="16">
         <f>G21/H21</f>
-        <v>0.61803398874989479</v>
+        <v>0.79056941504209477</v>
       </c>
       <c r="K21" s="12">
-        <v>4.803262507670838</v>
+        <v>4.4703563158921886</v>
       </c>
       <c r="L21" s="12">
-        <v>-1.8346830210422072</v>
+        <v>-2.2351781579460943</v>
       </c>
       <c r="M21" s="11"/>
       <c r="N21" s="12">
-        <v>4.4982058005029524</v>
+        <v>4.6619305189010118</v>
       </c>
       <c r="O21" s="12">
-        <v>-1.9591064880684124</v>
+        <v>-1.7146618131707518</v>
       </c>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.2">
       <c r="D22" s="12">
-        <v>-2.41778135780703</v>
+        <v>-2.8001715145991186</v>
       </c>
       <c r="E22" s="12">
-        <v>-2.8448358700263783</v>
+        <v>-2.73690837979166</v>
       </c>
       <c r="K22" s="12">
-        <v>3.9120524142976461</v>
+        <v>4.4274599126283238</v>
       </c>
       <c r="L22" s="12">
-        <v>-1.4942710564906152</v>
+        <v>-2.2137299563141619</v>
       </c>
       <c r="M22" s="11"/>
       <c r="N22" s="12">
-        <v>3.6635967394583147</v>
+        <v>4.6171958182651895</v>
       </c>
       <c r="O22" s="12">
-        <v>-1.5956086627109303</v>
+        <v>-1.6982083541170649</v>
       </c>
     </row>
     <row r="23" spans="2:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D23" s="12">
-        <v>-1.4437314527037302</v>
+        <v>-1.5953471421287813</v>
       </c>
       <c r="E23" s="12">
-        <v>-1.1014456258232872</v>
+        <v>-1.0980237762708427</v>
       </c>
       <c r="G23" s="21" t="s">
         <v>4</v>
       </c>
       <c r="H23" s="22"/>
       <c r="K23" s="12">
-        <v>2.3360065611018972</v>
+        <v>2.5224653138836564</v>
       </c>
       <c r="L23" s="12">
-        <v>-0.89227510839816637</v>
+        <v>-1.2612326569418282</v>
       </c>
       <c r="M23" s="11"/>
       <c r="N23" s="12">
-        <v>2.1876460523197365</v>
+        <v>2.6305639190008239</v>
       </c>
       <c r="O23" s="12">
-        <v>-0.9527869032176427</v>
+        <v>-0.96752353573875383</v>
       </c>
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.2">
       <c r="D24" s="12">
-        <v>-8.6752219445988987E-2</v>
+        <v>-2.1362449557817492E-2</v>
       </c>
       <c r="E24" s="12">
-        <v>0.51381735373193005</v>
+        <v>0.4547646281458928</v>
       </c>
       <c r="G24" s="13">
         <f t="array" ref="G24:H25">_xll.tdmLookup($D$5,$G$23)</f>
-        <v>0.83462956668806398</v>
+        <v>0.85504421295690458</v>
       </c>
       <c r="H24" s="14">
-        <v>0.55081166146886762</v>
+        <v>0.51855510207586164</v>
       </c>
       <c r="I24" s="15">
         <f>G24/H24</f>
-        <v>1.5152721430449199</v>
+        <v>1.6488975029539223</v>
       </c>
       <c r="K24" s="12">
-        <v>0.14036803966309977</v>
+        <v>3.3776998501580065E-2</v>
       </c>
       <c r="L24" s="12">
-        <v>-5.3615820217110761E-2</v>
+        <v>-1.6888499250790032E-2</v>
       </c>
       <c r="M24" s="11"/>
       <c r="N24" s="12">
-        <v>0.1314532214738269</v>
+        <v>3.5224489732864385E-2</v>
       </c>
       <c r="O24" s="12">
-        <v>-5.7251906757595054E-2</v>
+        <v>-1.2955595796310971E-2</v>
       </c>
     </row>
     <row r="25" spans="2:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D25" s="12">
-        <v>-1.1318578502408401</v>
+        <v>-0.97150846431236304</v>
       </c>
       <c r="E25" s="12">
-        <v>1.3102299358020968</v>
+        <v>1.0908230921970343</v>
       </c>
       <c r="G25" s="13">
-        <v>0.55081166146886762</v>
+        <v>-0.51855510207586164</v>
       </c>
       <c r="H25" s="14">
-        <v>-0.83462956668806398</v>
+        <v>0.85504421295690458</v>
       </c>
       <c r="I25" s="16">
         <f>G25/H25</f>
-        <v>-0.65994745867267968</v>
+        <v>-0.6064658344187841</v>
       </c>
       <c r="K25" s="12">
-        <v>1.8313844721230679</v>
+        <v>1.5360897566797374</v>
       </c>
       <c r="L25" s="12">
-        <v>-0.69952662188222747</v>
+        <v>-0.76804487833986868</v>
       </c>
       <c r="M25" s="11"/>
       <c r="N25" s="12">
-        <v>1.7150726703566537</v>
+        <v>1.6019178809032553</v>
       </c>
       <c r="O25" s="12">
-        <v>-0.74696671184516483</v>
+        <v>-0.58918669145410874</v>
       </c>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.2">
       <c r="D26" s="12">
-        <v>-1.3065842017830078</v>
+        <v>-1.3978832248512061</v>
       </c>
       <c r="E26" s="12">
-        <v>-0.639362708654165</v>
+        <v>-0.67278641135462713</v>
       </c>
       <c r="K26" s="12">
-        <v>2.114097647648558</v>
+        <v>2.2102474467355502</v>
       </c>
       <c r="L26" s="12">
-        <v>-0.80751344586554974</v>
+        <v>-1.1051237233677751</v>
       </c>
       <c r="M26" s="11"/>
       <c r="N26" s="12">
-        <v>1.9798306435043742</v>
+        <v>2.3049661588783299</v>
       </c>
       <c r="O26" s="12">
-        <v>-0.86227692350856777</v>
+        <v>-0.84776841637940747</v>
       </c>
     </row>
     <row r="27" spans="2:15" x14ac:dyDescent="0.2">
       <c r="D27" s="12">
-        <v>-0.92440787242906031</v>
+        <v>-0.94505207925248624</v>
       </c>
       <c r="E27" s="12">
-        <v>-0.11018890537115889</v>
+        <v>-0.1687943763747603</v>
       </c>
       <c r="K27" s="12">
-        <v>1.4957233570581967</v>
+        <v>1.4942585389579068</v>
       </c>
       <c r="L27" s="12">
-        <v>-0.57131548462913606</v>
+        <v>-0.74712926947895342</v>
       </c>
       <c r="M27" s="11"/>
       <c r="N27" s="12">
-        <v>1.400729497903177</v>
+        <v>1.558294013640837</v>
       </c>
       <c r="O27" s="12">
-        <v>-0.61006062618657697</v>
+        <v>-0.57314179781306596</v>
       </c>
     </row>
     <row r="28" spans="2:15" x14ac:dyDescent="0.2">
       <c r="D28" s="12">
-        <v>-2.2906759421687668</v>
+        <v>-2.5250236186137709</v>
       </c>
       <c r="E28" s="12">
-        <v>-1.6992373369234071</v>
+        <v>-1.6987485686757164</v>
       </c>
       <c r="K28" s="12">
-        <v>3.7063915316407536</v>
+        <v>3.9924128902699243</v>
       </c>
       <c r="L28" s="12">
-        <v>-1.4157155894719862</v>
+        <v>-1.9962064451349621</v>
       </c>
       <c r="M28" s="11"/>
       <c r="N28" s="12">
-        <v>3.4709974439115081</v>
+        <v>4.1635051396319236</v>
       </c>
       <c r="O28" s="12">
-        <v>-1.5117257666769237</v>
+        <v>-1.5313405557897382</v>
       </c>
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.2">
       <c r="D29" s="12">
-        <v>2.1306014483965074E-2</v>
+        <v>-0.1284643813395443</v>
       </c>
       <c r="E29" s="12">
-        <v>-1.1671634409526259</v>
+        <v>-1.0463050536852585</v>
       </c>
       <c r="K29" s="12">
-        <v>-3.4473855599853047E-2</v>
+        <v>0.20312002161869627</v>
       </c>
       <c r="L29" s="12">
-        <v>1.3167841115887965E-2</v>
+        <v>-0.10156001080934814</v>
       </c>
       <c r="M29" s="11"/>
       <c r="N29" s="12">
-        <v>-3.2284410226863861E-2</v>
+        <v>0.21182459760929506</v>
       </c>
       <c r="O29" s="12">
-        <v>1.4060850113136056E-2</v>
+        <v>-7.7909258222179617E-2</v>
       </c>
     </row>
     <row r="30" spans="2:15" x14ac:dyDescent="0.2">
       <c r="D30" s="12">
-        <v>3.7268657872907642</v>
+        <v>4.1649165765948473</v>
       </c>
       <c r="E30" s="12">
-        <v>3.2066084112744391</v>
+        <v>3.1606547474661997</v>
       </c>
       <c r="K30" s="12">
-        <v>-6.0301955153455937</v>
+        <v>-6.585311323315425</v>
       </c>
       <c r="L30" s="12">
-        <v>2.3033297280548282</v>
+        <v>3.2926556616577125</v>
       </c>
       <c r="M30" s="11"/>
       <c r="N30" s="12">
-        <v>-5.6472159083488691</v>
+        <v>-6.8675205431586424</v>
       </c>
       <c r="O30" s="12">
-        <v>2.4595356051366952</v>
+        <v>2.52587960690922</v>
       </c>
     </row>
     <row r="31" spans="2:15" x14ac:dyDescent="0.2">
       <c r="D31" s="12">
-        <v>-0.94000394298800316</v>
+        <v>-1.1529690614774375</v>
       </c>
       <c r="E31" s="12">
-        <v>-1.6066012192659476</v>
+        <v>-1.513498134033016</v>
       </c>
       <c r="K31" s="12">
-        <v>1.5209583293135078</v>
+        <v>1.8230041529877015</v>
       </c>
       <c r="L31" s="12">
-        <v>-0.58095438632550433</v>
+        <v>-0.91150207649385073</v>
       </c>
       <c r="M31" s="11"/>
       <c r="N31" s="12">
-        <v>1.4243617891621063</v>
+        <v>1.9011278064532742</v>
       </c>
       <c r="O31" s="12">
-        <v>-0.62035321331723114</v>
+        <v>-0.69923634392795653</v>
       </c>
     </row>
     <row r="32" spans="2:15" x14ac:dyDescent="0.2">
       <c r="D32" s="12">
-        <v>-2.7736927087609806</v>
+        <v>-3.2715243295705934</v>
       </c>
       <c r="E32" s="12">
-        <v>-3.7241202985863722</v>
+        <v>-3.5532555056976376</v>
       </c>
       <c r="K32" s="12">
-        <v>4.4879290771230309</v>
+        <v>5.1727341510492106</v>
       </c>
       <c r="L32" s="12">
-        <v>-1.7142363683620492</v>
+        <v>-2.5863670755246053</v>
       </c>
       <c r="M32" s="11"/>
       <c r="N32" s="12">
-        <v>4.2028992949523198</v>
+        <v>5.3944082978819559</v>
       </c>
       <c r="O32" s="12">
-        <v>-1.8304914542857502</v>
+        <v>-1.9840677323543832</v>
       </c>
     </row>
     <row r="33" spans="4:15" x14ac:dyDescent="0.2">
       <c r="D33" s="12">
-        <v>4.1647145192488161E-2</v>
+        <v>1.2018548796580736E-2</v>
       </c>
       <c r="E33" s="12">
-        <v>-0.23294236732727963</v>
+        <v>-0.20599529207929601</v>
       </c>
       <c r="K33" s="12">
-        <v>-6.7386496455847641E-2</v>
+        <v>-1.9002994183535408E-2</v>
       </c>
       <c r="L33" s="12">
-        <v>2.5739351263359463E-2</v>
+        <v>9.5014970917677039E-3</v>
       </c>
       <c r="M33" s="11"/>
       <c r="N33" s="12">
-        <v>-6.3106758947524461E-2</v>
+        <v>-1.9817355099811845E-2</v>
       </c>
       <c r="O33" s="12">
-        <v>2.748492763075467E-2</v>
+        <v>7.2888392244212091E-3</v>
       </c>
     </row>
     <row r="34" spans="4:15" x14ac:dyDescent="0.2">
       <c r="D34" s="12">
-        <v>-3.388202527547457</v>
+        <v>-3.4201387193997577</v>
       </c>
       <c r="E34" s="12">
-        <v>-6.3420444458172742E-2</v>
+        <v>-0.31300884695931019</v>
       </c>
       <c r="K34" s="12">
-        <v>5.4822268503400879</v>
+        <v>5.4077141335173708</v>
       </c>
       <c r="L34" s="12">
-        <v>-2.0940243227926301</v>
+        <v>-2.7038570667586854</v>
       </c>
       <c r="M34" s="11"/>
       <c r="N34" s="12">
-        <v>5.1340489049870497</v>
+        <v>5.6394581941742858</v>
       </c>
       <c r="O34" s="12">
-        <v>-2.2360356475232943</v>
+        <v>-2.0741972822887655</v>
       </c>
     </row>
     <row r="35" spans="4:15" x14ac:dyDescent="0.2">
       <c r="D35" s="12">
-        <v>-0.48442749163235099</v>
+        <v>-0.45915728708917769</v>
       </c>
       <c r="E35" s="12">
-        <v>0.22321509390525715</v>
+        <v>0.16379811893780888</v>
       </c>
       <c r="K35" s="12">
-        <v>0.7838201465459993</v>
+        <v>0.72599141573281278</v>
       </c>
       <c r="L35" s="12">
-        <v>-0.29939265491364819</v>
+        <v>-0.36299570786640639</v>
       </c>
       <c r="M35" s="11"/>
       <c r="N35" s="12">
-        <v>0.73403948339562752</v>
+        <v>0.75710330414444238</v>
       </c>
       <c r="O35" s="12">
-        <v>-0.31969669201395085</v>
+        <v>-0.27846320724400336</v>
       </c>
     </row>
     <row r="36" spans="4:15" x14ac:dyDescent="0.2">
       <c r="D36" s="12">
-        <v>2.6606670565513966</v>
+        <v>2.5389534719981048</v>
       </c>
       <c r="E36" s="12">
-        <v>-1.0930107205938138</v>
+        <v>-0.78025515359969366</v>
       </c>
       <c r="K36" s="12">
-        <v>-4.3050497302472985</v>
+        <v>-4.0144379223532747</v>
       </c>
       <c r="L36" s="12">
-        <v>1.6443826736959015</v>
+        <v>2.0072189611766373</v>
       </c>
       <c r="M36" s="11"/>
       <c r="N36" s="12">
-        <v>-4.0316346727096537</v>
+        <v>-4.1864740400938665</v>
       </c>
       <c r="O36" s="12">
-        <v>1.755900462345213</v>
+        <v>1.5397885359457997</v>
       </c>
     </row>
     <row r="37" spans="4:15" x14ac:dyDescent="0.2">
       <c r="D37" s="12">
-        <v>0.46630470569647697</v>
+        <v>0.53435023312261143</v>
       </c>
       <c r="E37" s="12">
-        <v>0.50426111843013266</v>
+        <v>0.48798277580607641</v>
       </c>
       <c r="K37" s="12">
-        <v>-0.75449686293091656</v>
+        <v>-0.84488190245469974</v>
       </c>
       <c r="L37" s="12">
-        <v>0.28819215723443947</v>
+        <v>0.42244095122734987</v>
       </c>
       <c r="M37" s="11"/>
       <c r="N37" s="12">
-        <v>-0.70657853071263133</v>
+        <v>-0.88108876509872025</v>
       </c>
       <c r="O37" s="12">
-        <v>0.30773660549150178</v>
+        <v>0.32406516000257635</v>
       </c>
     </row>
     <row r="38" spans="4:15" x14ac:dyDescent="0.2">
       <c r="D38" s="12">
-        <v>-2.7337637513964221</v>
+        <v>-2.7565437172239053</v>
       </c>
       <c r="E38" s="12">
-        <v>-2.7910831943309677E-2</v>
+        <v>-0.23166712173813697</v>
       </c>
       <c r="K38" s="12">
-        <v>4.4233226669718295</v>
+        <v>4.3584783081273288</v>
       </c>
       <c r="L38" s="12">
-        <v>-1.6895589155754065</v>
+        <v>-2.1792391540636644</v>
       </c>
       <c r="M38" s="11"/>
       <c r="N38" s="12">
-        <v>4.1423960581569759</v>
+        <v>4.5452580521138204</v>
       </c>
       <c r="O38" s="12">
-        <v>-1.8041404403455601</v>
+        <v>-1.6717495855780526</v>
       </c>
     </row>
     <row r="39" spans="4:15" x14ac:dyDescent="0.2">
       <c r="D39" s="12">
-        <v>0.81354133006853036</v>
+        <v>0.83017472050027152</v>
       </c>
       <c r="E39" s="12">
-        <v>8.5024066832616763E-2</v>
+        <v>0.13782171941336896</v>
       </c>
       <c r="K39" s="12">
-        <v>-1.3163375233036791</v>
+        <v>-1.3126214863372683</v>
       </c>
       <c r="L39" s="12">
-        <v>0.50279619323514857</v>
+        <v>0.65631074316863414</v>
       </c>
       <c r="M39" s="11"/>
       <c r="N39" s="12">
-        <v>-1.2327365146685565</v>
+        <v>-1.3688730236483682</v>
       </c>
       <c r="O39" s="12">
-        <v>0.53689453330391834</v>
+        <v>0.50347260458157805</v>
       </c>
     </row>
     <row r="40" spans="4:15" x14ac:dyDescent="0.2">
       <c r="D40" s="12">
-        <v>2.5742136862941565</v>
+        <v>2.5445742996357965</v>
       </c>
       <c r="E40" s="12">
-        <v>-0.37146497211188234</v>
+        <v>-0.13896298888945968</v>
       </c>
       <c r="K40" s="12">
-        <v>-4.1651652387291049</v>
+        <v>-4.0233252311884389</v>
       </c>
       <c r="L40" s="12">
-        <v>1.590951552434948</v>
+        <v>2.0116626155942194</v>
       </c>
       <c r="M40" s="11"/>
       <c r="N40" s="12">
-        <v>-3.9006342890865096</v>
+        <v>-4.1957422087501905</v>
       </c>
       <c r="O40" s="12">
-        <v>1.6988457803502592</v>
+        <v>1.5431973758692166</v>
       </c>
     </row>
     <row r="41" spans="4:15" x14ac:dyDescent="0.2">
       <c r="D41" s="12">
-        <v>1.5551576637517777</v>
+        <v>2.035817829460961</v>
       </c>
       <c r="E41" s="12">
-        <v>3.6570455858568018</v>
+        <v>3.4009413178641887</v>
       </c>
       <c r="K41" s="12">
-        <v>-2.5162979578152571</v>
+        <v>-3.2189106211384382</v>
       </c>
       <c r="L41" s="12">
-        <v>0.96114029406347878</v>
+        <v>1.6094553105692191</v>
       </c>
       <c r="M41" s="11"/>
       <c r="N41" s="12">
-        <v>-2.3564870859258868</v>
+        <v>-3.3568549354672528</v>
       </c>
       <c r="O41" s="12">
-        <v>1.0263223480283274</v>
+        <v>1.2346539586686796</v>
       </c>
     </row>
     <row r="42" spans="4:15" x14ac:dyDescent="0.2">
       <c r="D42" s="12">
-        <v>1.0953793605083002</v>
+        <v>1.11226451285018</v>
       </c>
       <c r="E42" s="12">
-        <v>7.1577880140467232E-2</v>
+        <v>0.14704961171049302</v>
       </c>
       <c r="K42" s="12">
-        <v>-1.7723610358775543</v>
+        <v>-1.7586446105920945</v>
       </c>
       <c r="L42" s="12">
-        <v>0.6769816753692538</v>
+        <v>0.87932230529604727</v>
       </c>
       <c r="M42" s="11"/>
       <c r="N42" s="12">
-        <v>-1.659797831044586</v>
+        <v>-1.8340101778629228</v>
       </c>
       <c r="O42" s="12">
-        <v>0.72289282524995779</v>
+        <v>0.67455042588008685</v>
       </c>
     </row>
     <row r="43" spans="4:15" x14ac:dyDescent="0.2">
       <c r="D43" s="12">
-        <v>1.5465500076795724</v>
+        <v>1.8181954267576632</v>
       </c>
       <c r="E43" s="12">
-        <v>2.0302857158818362</v>
+        <v>1.9397356687235576</v>
       </c>
       <c r="K43" s="12">
-        <v>-2.5023704777269593</v>
+        <v>-2.8748193899280352</v>
       </c>
       <c r="L43" s="12">
-        <v>0.95582047004738657</v>
+        <v>1.4374096949640176</v>
       </c>
       <c r="M43" s="11"/>
       <c r="N43" s="12">
-        <v>-2.3434441444627629</v>
+        <v>-2.998017899062952</v>
       </c>
       <c r="O43" s="12">
-        <v>1.0206417472783471</v>
+        <v>1.1026734066250035</v>
       </c>
     </row>
     <row r="44" spans="4:15" x14ac:dyDescent="0.2">
       <c r="D44" s="12">
-        <v>2.7428222956674717</v>
+        <v>2.9420568788376582</v>
       </c>
       <c r="E44" s="12">
-        <v>1.4011575673439829</v>
+        <v>1.4652949472004522</v>
       </c>
       <c r="K44" s="12">
-        <v>-4.4379796994909837</v>
+        <v>-4.6518003714465168</v>
       </c>
       <c r="L44" s="12">
-        <v>1.6951574038235109</v>
+        <v>2.3259001857232584</v>
       </c>
       <c r="M44" s="11"/>
       <c r="N44" s="12">
-        <v>-4.1561222179474369</v>
+        <v>-4.8511502410638254</v>
       </c>
       <c r="O44" s="12">
-        <v>1.8101186036165131</v>
+        <v>1.784256979931804</v>
       </c>
     </row>
     <row r="45" spans="4:15" x14ac:dyDescent="0.2">
       <c r="D45" s="12">
-        <v>1.2097764377910976</v>
+        <v>1.3829887153182421</v>
       </c>
       <c r="E45" s="12">
-        <v>1.2823690590529375</v>
+        <v>1.2427809381294084</v>
       </c>
       <c r="K45" s="12">
-        <v>-1.957459395134769</v>
+        <v>-2.1866971593579216</v>
       </c>
       <c r="L45" s="12">
-        <v>0.74768295734367096</v>
+        <v>1.0933485796789608</v>
       </c>
       <c r="M45" s="11"/>
       <c r="N45" s="12">
-        <v>-1.8331405354969657</v>
+        <v>-2.2804066393017024</v>
       </c>
       <c r="O45" s="12">
-        <v>0.79838888568232202</v>
+        <v>0.83873540522723999</v>
       </c>
     </row>
     <row r="46" spans="4:15" x14ac:dyDescent="0.2">
       <c r="D46" s="12">
-        <v>1.556170892214177</v>
+        <v>1.4810593527901463</v>
       </c>
       <c r="E46" s="12">
-        <v>-0.66982704655353886</v>
+        <v>-0.48378161867430658</v>
       </c>
       <c r="K46" s="12">
-        <v>-2.517937395905788</v>
+        <v>-2.3417604523558588</v>
       </c>
       <c r="L46" s="12">
-        <v>0.96176650369161043</v>
+        <v>1.1708802261779294</v>
       </c>
       <c r="M46" s="11"/>
       <c r="N46" s="12">
-        <v>-2.3580224027895009</v>
+        <v>-2.4421150685422246</v>
       </c>
       <c r="O46" s="12">
-        <v>1.0269910255771426</v>
+        <v>0.89821189621362041</v>
       </c>
     </row>
     <row r="47" spans="4:15" x14ac:dyDescent="0.2">
       <c r="D47" s="12">
-        <v>-0.21912385112196342</v>
+        <v>-0.16202401401030964</v>
       </c>
       <c r="E47" s="12">
-        <v>0.4565140988690724</v>
+        <v>0.39331183477641812</v>
       </c>
       <c r="K47" s="12">
-        <v>0.35454983886110863</v>
+        <v>0.25618245995780531</v>
       </c>
       <c r="L47" s="12">
-        <v>-0.13542598773914516</v>
+        <v>-0.12809122997890265</v>
       </c>
       <c r="M47" s="11"/>
       <c r="N47" s="12">
-        <v>0.33203226748183345</v>
+        <v>0.26716099212017091</v>
       </c>
       <c r="O47" s="12">
-        <v>-0.14461022868251036</v>
+        <v>-9.8262028852643193E-2</v>
       </c>
     </row>
     <row r="48" spans="4:15" x14ac:dyDescent="0.2">
       <c r="D48" s="12">
-        <v>-0.29456504009806828</v>
+        <v>-0.26632535803392365</v>
       </c>
       <c r="E48" s="12">
-        <v>0.23595467535661346</v>
+        <v>0.18958522078003032</v>
       </c>
       <c r="K48" s="12">
-        <v>0.47661624677615022</v>
+        <v>0.42109736502351097</v>
       </c>
       <c r="L48" s="12">
-        <v>-0.18205120667808183</v>
+        <v>-0.21054868251175549</v>
       </c>
       <c r="M48" s="11"/>
       <c r="N48" s="12">
-        <v>0.44634619957551269</v>
+        <v>0.43914321783544608</v>
       </c>
       <c r="O48" s="12">
-        <v>-0.19439744962653616</v>
+        <v>-0.16151723048692493</v>
       </c>
     </row>
     <row r="49" spans="4:15" x14ac:dyDescent="0.2">
       <c r="D49" s="12">
-        <v>1.2505410770896126</v>
+        <v>1.2942057062086234</v>
       </c>
       <c r="E49" s="12">
-        <v>0.27158092769382552</v>
+        <v>0.33834506565874178</v>
       </c>
       <c r="K49" s="12">
-        <v>-2.0234179670588959</v>
+        <v>-2.046318896202985</v>
       </c>
       <c r="L49" s="12">
-        <v>0.77287688996928294</v>
+        <v>1.0231594481014925</v>
       </c>
       <c r="M49" s="11"/>
       <c r="N49" s="12">
-        <v>-1.8949100578472795</v>
+        <v>-2.1340125572761166</v>
       </c>
       <c r="O49" s="12">
-        <v>0.8252914057910854</v>
+        <v>0.7848915435253645</v>
       </c>
     </row>
     <row r="50" spans="4:15" x14ac:dyDescent="0.2">
       <c r="D50" s="12">
-        <v>1.3102799351859984</v>
+        <v>1.3596723098360501</v>
       </c>
       <c r="E50" s="12">
-        <v>0.31290728623540981</v>
+        <v>0.3799639886949574</v>
       </c>
       <c r="K50" s="12">
-        <v>-2.120077469907955</v>
+        <v>-2.1498306852720401</v>
       </c>
       <c r="L50" s="12">
-        <v>0.80979753472195626</v>
+        <v>1.0749153426360201</v>
       </c>
       <c r="M50" s="11"/>
       <c r="N50" s="12">
-        <v>-1.9854306853780466</v>
+        <v>-2.2419602765242548</v>
       </c>
       <c r="O50" s="12">
-        <v>0.86471591337580311</v>
+        <v>0.82459480192083567</v>
       </c>
     </row>
     <row r="51" spans="4:15" x14ac:dyDescent="0.2">
       <c r="D51" s="12">
-        <v>2.3825996446021298</v>
+        <v>2.2820381706635873</v>
       </c>
       <c r="E51" s="12">
-        <v>-0.91313632028722236</v>
+        <v>-0.63977370026823366</v>
       </c>
       <c r="K51" s="12">
-        <v>-3.8551272065496667</v>
+        <v>-3.6082191633704883</v>
       </c>
       <c r="L51" s="12">
-        <v>1.472527561947536</v>
+        <v>1.8041095816852442</v>
       </c>
       <c r="M51" s="11"/>
       <c r="N51" s="12">
-        <v>-3.6102868694943338</v>
+        <v>-3.762847041252726</v>
       </c>
       <c r="O51" s="12">
-        <v>1.5723905804896054</v>
+        <v>1.3839781833470082</v>
       </c>
     </row>
     <row r="52" spans="4:15" x14ac:dyDescent="0.2">
       <c r="D52" s="12">
-        <v>-3.8767254050886851E-2</v>
+        <v>-0.11343753707577428</v>
       </c>
       <c r="E52" s="12">
-        <v>-0.57920707846201458</v>
+        <v>-0.52295984203446566</v>
       </c>
       <c r="K52" s="12">
-        <v>6.2726734704836987E-2</v>
+        <v>0.17936049465962162</v>
       </c>
       <c r="L52" s="12">
-        <v>-2.3959480653950118E-2</v>
+        <v>-8.9680247329810808E-2</v>
       </c>
       <c r="M52" s="11"/>
       <c r="N52" s="12">
-        <v>5.8742940125654168E-2</v>
+        <v>0.18704687162548719</v>
       </c>
       <c r="O52" s="12">
-        <v>-2.5584350790600924E-2</v>
+        <v>-6.8795990577071212E-2</v>
       </c>
     </row>
     <row r="53" spans="4:15" x14ac:dyDescent="0.2">
       <c r="D53" s="12">
-        <v>2.3517011704896866</v>
+        <v>2.6370529271427077</v>
       </c>
       <c r="E53" s="12">
-        <v>2.0929806024918185</v>
+        <v>2.0568754641042482</v>
       </c>
       <c r="K53" s="12">
-        <v>-3.8051324252352248</v>
+        <v>-4.1695467800925083</v>
       </c>
       <c r="L53" s="12">
-        <v>1.4534312547455375</v>
+        <v>2.0847733900462542</v>
       </c>
       <c r="M53" s="11"/>
       <c r="N53" s="12">
-        <v>-3.5634672724091541</v>
+        <v>-4.3482299867229424</v>
       </c>
       <c r="O53" s="12">
-        <v>1.5519992110222349</v>
+        <v>1.5992825038660994</v>
       </c>
     </row>
     <row r="54" spans="4:15" x14ac:dyDescent="0.2">
       <c r="D54" s="12">
-        <v>1.4359355713481932</v>
+        <v>1.5692309550064412</v>
       </c>
       <c r="E54" s="12">
-        <v>0.95924376017938107</v>
+        <v>0.96976137727618472</v>
       </c>
       <c r="K54" s="12">
-        <v>-2.3233925600963765</v>
+        <v>-2.4811719963307799</v>
       </c>
       <c r="L54" s="12">
-        <v>0.88745698874818302</v>
+        <v>1.2405859981653899</v>
       </c>
       <c r="M54" s="11"/>
       <c r="N54" s="12">
-        <v>-2.1758331704712082</v>
+        <v>-2.5875010032681196</v>
       </c>
       <c r="O54" s="12">
-        <v>0.94764203112894241</v>
+        <v>0.95168496052376683</v>
       </c>
     </row>
     <row r="55" spans="4:15" x14ac:dyDescent="0.2">
       <c r="D55" s="12">
-        <v>-1.2594091332959976</v>
+        <v>-1.3453346811645239</v>
       </c>
       <c r="E55" s="12">
-        <v>-0.60010765142012623</v>
+        <v>-0.6339766919300811</v>
       </c>
       <c r="K55" s="12">
-        <v>2.0377667834149715</v>
+        <v>2.1271609038481616</v>
       </c>
       <c r="L55" s="12">
-        <v>-0.77835765011897329</v>
+        <v>-1.0635804519240808</v>
       </c>
       <c r="M55" s="11"/>
       <c r="N55" s="12">
-        <v>1.9083475763797715</v>
+        <v>2.2183189964094949</v>
       </c>
       <c r="O55" s="12">
-        <v>-0.83114385694785564</v>
+        <v>-0.8158995199849719</v>
       </c>
     </row>
     <row r="56" spans="4:15" x14ac:dyDescent="0.2">
       <c r="D56" s="12">
-        <v>-1.0804247072314288</v>
+        <v>-1.3929758311627096</v>
       </c>
       <c r="E56" s="12">
-        <v>-2.3742265048969529</v>
+        <v>-2.2133082479746728</v>
       </c>
       <c r="K56" s="12">
-        <v>1.7481638985856065</v>
+        <v>2.2024881760201582</v>
       </c>
       <c r="L56" s="12">
-        <v>-0.66773919135417725</v>
+        <v>-1.1012440880100791</v>
       </c>
       <c r="M56" s="11"/>
       <c r="N56" s="12">
-        <v>1.6371374615252472</v>
+        <v>2.2968743696793563</v>
       </c>
       <c r="O56" s="12">
-        <v>-0.71302353982455535</v>
+        <v>-0.84479224977129197</v>
       </c>
     </row>
     <row r="57" spans="4:15" x14ac:dyDescent="0.2">
       <c r="D57" s="12">
-        <v>-0.22776653847466866</v>
+        <v>-0.36900841771634313</v>
       </c>
       <c r="E57" s="12">
-        <v>-1.0871517321178621</v>
+        <v>-0.99329207448549706</v>
       </c>
       <c r="K57" s="12">
-        <v>0.36853400075192461</v>
+        <v>0.58345353787923671</v>
       </c>
       <c r="L57" s="12">
-        <v>-0.14076746227725584</v>
+        <v>-0.29172676893961835</v>
       </c>
       <c r="M57" s="11"/>
       <c r="N57" s="12">
-        <v>0.34512829086843438</v>
+        <v>0.60845705854145615</v>
       </c>
       <c r="O57" s="12">
-        <v>-0.1503139482370307</v>
+        <v>-0.22379099795789728</v>
       </c>
     </row>
     <row r="58" spans="4:15" x14ac:dyDescent="0.2">
       <c r="D58" s="12">
-        <v>1.7667281518836884</v>
+        <v>1.8166331877928579</v>
       </c>
       <c r="E58" s="12">
-        <v>0.29194748441746643</v>
+        <v>0.39564232845712016</v>
       </c>
       <c r="K58" s="12">
-        <v>-2.8586261986290946</v>
+        <v>-2.8723492732389109</v>
       </c>
       <c r="L58" s="12">
-        <v>1.0918980467454058</v>
+        <v>1.4361746366194554</v>
       </c>
       <c r="M58" s="11"/>
       <c r="N58" s="12">
-        <v>-2.6770739528825871</v>
+        <v>-2.9954419271348671</v>
       </c>
       <c r="O58" s="12">
-        <v>1.1659477540011203</v>
+        <v>1.1017259620676512</v>
       </c>
     </row>
     <row r="59" spans="4:15" x14ac:dyDescent="0.2">
       <c r="D59" s="12">
-        <v>0.46939049577543013</v>
+        <v>0.51991896160788809</v>
       </c>
       <c r="E59" s="12">
-        <v>0.36771787435711811</v>
+        <v>0.36562325867027584</v>
       </c>
       <c r="K59" s="12">
-        <v>-0.75948977616081004</v>
+        <v>-0.82206405869528287</v>
       </c>
       <c r="L59" s="12">
-        <v>0.29009928038537974</v>
+        <v>0.41103202934764144</v>
       </c>
       <c r="M59" s="11"/>
       <c r="N59" s="12">
-        <v>-0.71125434245855346</v>
+        <v>-0.85729307753364292</v>
       </c>
       <c r="O59" s="12">
-        <v>0.30977306481210432</v>
+        <v>0.31531308688167564</v>
       </c>
     </row>
     <row r="60" spans="4:15" x14ac:dyDescent="0.2">
       <c r="D60" s="12">
-        <v>1.3285106574701482</v>
+        <v>1.6032095266440509</v>
       </c>
       <c r="E60" s="12">
-        <v>2.0659763277375434</v>
+        <v>1.9553011785564176</v>
       </c>
       <c r="K60" s="12">
-        <v>-2.1495753982031696</v>
+        <v>-2.5348968353378019</v>
       </c>
       <c r="L60" s="12">
-        <v>0.82106474073302094</v>
+        <v>1.2674484176689009</v>
       </c>
       <c r="M60" s="11"/>
       <c r="N60" s="12">
-        <v>-2.0130551910028069</v>
+        <v>-2.6435281851953154</v>
       </c>
       <c r="O60" s="12">
-        <v>0.87674723221699513</v>
+        <v>0.97229180332432819</v>
       </c>
     </row>
     <row r="61" spans="4:15" x14ac:dyDescent="0.2">
       <c r="D61" s="12">
-        <v>0.19599315835367093</v>
+        <v>-5.977184802549973E-2</v>
       </c>
       <c r="E61" s="12">
-        <v>-2.0019061260076834</v>
+        <v>-1.7825605268413125</v>
       </c>
       <c r="K61" s="12">
-        <v>-0.31712359177867999</v>
+        <v>9.4507589859008617E-2</v>
       </c>
       <c r="L61" s="12">
-        <v>0.12113043342500901</v>
+        <v>-4.7253794929504309E-2</v>
       </c>
       <c r="M61" s="11"/>
       <c r="N61" s="12">
-        <v>-0.29698297308070926</v>
+        <v>9.8557650956187834E-2</v>
       </c>
       <c r="O61" s="12">
-        <v>0.12934518677273721</v>
+        <v>-3.6249583687537446E-2</v>
       </c>
     </row>
     <row r="62" spans="4:15" x14ac:dyDescent="0.2">
       <c r="D62" s="12">
-        <v>-3.5797665830828085</v>
+        <v>-3.5525413655823783</v>
       </c>
       <c r="E62" s="12">
-        <v>0.40763698223498301</v>
+        <v>9.5443304528013861E-2</v>
       </c>
       <c r="K62" s="12">
-        <v>5.7921840032190595</v>
+        <v>5.617061098602611</v>
       </c>
       <c r="L62" s="12">
-        <v>-2.2124174201362496</v>
+        <v>-2.8085305493013055</v>
       </c>
       <c r="M62" s="11"/>
       <c r="N62" s="12">
-        <v>5.4243205819484777</v>
+        <v>5.857776586849301</v>
       </c>
       <c r="O62" s="12">
-        <v>-2.3624578591468817</v>
+        <v>-2.1544949635851638</v>
       </c>
     </row>
     <row r="63" spans="4:15" x14ac:dyDescent="0.2">
       <c r="D63" s="12">
-        <v>-1.7961057474280631</v>
+        <v>-1.9832400171325459</v>
       </c>
       <c r="E63" s="12">
-        <v>-1.3587044069720016</v>
+        <v>-1.3556298003331999</v>
       </c>
       <c r="K63" s="12">
-        <v>2.9061601467276406</v>
+        <v>3.1357778004651018</v>
       </c>
       <c r="L63" s="12">
-        <v>-1.1100543992995768</v>
+        <v>-1.5678889002325509</v>
       </c>
       <c r="M63" s="11"/>
       <c r="N63" s="12">
-        <v>2.7215890050406188</v>
+        <v>3.2701595120081492</v>
       </c>
       <c r="O63" s="12">
-        <v>-1.1853354235225442</v>
+        <v>-1.2027673118430131</v>
       </c>
     </row>
     <row r="64" spans="4:15" x14ac:dyDescent="0.2">
       <c r="D64" s="12">
-        <v>1.0808271284076445</v>
+        <v>1.3613946406106843</v>
       </c>
       <c r="E64" s="12">
-        <v>2.1252043484416792</v>
+        <v>1.9897588998079581</v>
       </c>
       <c r="K64" s="12">
-        <v>-1.7488150297265161</v>
+        <v>-2.1525539293380631</v>
       </c>
       <c r="L64" s="12">
-        <v>0.6679879013188712</v>
+        <v>1.0762769646690316</v>
       </c>
       <c r="M64" s="11"/>
       <c r="N64" s="12">
-        <v>-1.6377472391233383</v>
+        <v>-2.2448002234378097</v>
       </c>
       <c r="O64" s="12">
-        <v>0.71328911665711503</v>
+        <v>0.82563933669121936</v>
       </c>
     </row>
     <row r="65" spans="4:15" x14ac:dyDescent="0.2">
       <c r="D65" s="12">
-        <v>-0.10315859919307868</v>
+        <v>0.10492523587787572</v>
       </c>
       <c r="E65" s="12">
-        <v>1.6256220173556069</v>
+        <v>1.4517371631166123</v>
       </c>
       <c r="K65" s="12">
-        <v>0.1669141197262288</v>
+        <v>-0.16590136470225206</v>
       </c>
       <c r="L65" s="12">
-        <v>-6.375552053315009E-2</v>
+        <v>8.2950682351126029E-2</v>
       </c>
       <c r="M65" s="11"/>
       <c r="N65" s="12">
-        <v>0.15631335167280827</v>
+        <v>-0.17301095943588057</v>
       </c>
       <c r="O65" s="12">
-        <v>-6.8079255377705816E-2</v>
+        <v>6.3633570728263644E-2</v>
       </c>
     </row>
     <row r="66" spans="4:15" x14ac:dyDescent="0.2">
       <c r="D66" s="12">
-        <v>-0.94059211282138211</v>
+        <v>-0.84850144592058085</v>
       </c>
       <c r="E66" s="12">
-        <v>0.76836405840685229</v>
+        <v>0.6187743870433039</v>
       </c>
       <c r="K66" s="12">
-        <v>1.5219100080950723</v>
+        <v>1.3415985835276105</v>
       </c>
       <c r="L66" s="12">
-        <v>-0.58131789527368982</v>
+        <v>-0.67079929176380526</v>
       </c>
       <c r="M66" s="11"/>
       <c r="N66" s="12">
-        <v>1.4252530265260046</v>
+        <v>1.3990919154312385</v>
       </c>
       <c r="O66" s="12">
-        <v>-0.62074137450403755</v>
+        <v>-0.51458713740576989</v>
       </c>
     </row>
     <row r="67" spans="4:15" x14ac:dyDescent="0.2">
       <c r="D67" s="12">
-        <v>-1.0132991765578467</v>
+        <v>-0.97543054893021364</v>
       </c>
       <c r="E67" s="12">
-        <v>0.35020677101754616</v>
+        <v>0.23784496028199742</v>
       </c>
       <c r="K67" s="12">
-        <v>1.639552508442877</v>
+        <v>1.5422911169638969</v>
       </c>
       <c r="L67" s="12">
-        <v>-0.62625333188502985</v>
+        <v>-0.77114555848194843</v>
       </c>
       <c r="M67" s="11"/>
       <c r="N67" s="12">
-        <v>1.535424014808461</v>
+        <v>1.6083849964360031</v>
       </c>
       <c r="O67" s="12">
-        <v>-0.66872421644446989</v>
+        <v>-0.59156530177453459</v>
       </c>
     </row>
     <row r="68" spans="4:15" x14ac:dyDescent="0.2">
       <c r="D68" s="12">
-        <v>-1.1207180551482334</v>
+        <v>-0.90054400694640813</v>
       </c>
       <c r="E68" s="12">
-        <v>1.7753704731850142</v>
+        <v>1.5092824976949624</v>
       </c>
       <c r="K68" s="12">
-        <v>1.8133599050355211</v>
+        <v>1.4238850975825721</v>
       </c>
       <c r="L68" s="12">
-        <v>-0.69264184988728728</v>
+        <v>-0.71194254879128605</v>
       </c>
       <c r="M68" s="11"/>
       <c r="N68" s="12">
-        <v>1.6981928491735983</v>
+        <v>1.4849047643540521</v>
       </c>
       <c r="O68" s="12">
-        <v>-0.73961503238366466</v>
+        <v>-0.54614917260358875</v>
       </c>
     </row>
     <row r="69" spans="4:15" x14ac:dyDescent="0.2">
       <c r="D69" s="12">
-        <v>-0.45379116930259467</v>
+        <v>-0.42164425355533997</v>
       </c>
       <c r="E69" s="12">
-        <v>0.27507727074108163</v>
+        <v>0.21267696037101397</v>
       </c>
       <c r="K69" s="12">
-        <v>0.73424953572615625</v>
+        <v>0.66667810177821163</v>
       </c>
       <c r="L69" s="12">
-        <v>-0.28045836642356137</v>
+        <v>-0.33333905088910581</v>
       </c>
       <c r="M69" s="11"/>
       <c r="N69" s="12">
-        <v>0.68761711760400268</v>
+        <v>0.69524815682227059</v>
       </c>
       <c r="O69" s="12">
-        <v>-0.29947832894935106</v>
+        <v>-0.25571283406032463</v>
       </c>
     </row>
     <row r="70" spans="4:15" x14ac:dyDescent="0.2">

</xml_diff>